<commit_message>
Il worksheet dell'excel del grafico ora resta disattivo fino alla fine per evitare rallentamenti significativi
</commit_message>
<xml_diff>
--- a/ProgettoFormLetturaDati/HydrogenOMB/bin/Debug/File/base.xlsx
+++ b/ProgettoFormLetturaDati/HydrogenOMB/bin/Debug/File/base.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\principale\source\repos\ProgettoOMBCorreggiuto\ProgettoFormLetturaDati\HydrogenOMB\bin\Debug\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D01837C-B0AC-4BA7-AE34-AAE757E2742C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58CCC76-A87D-4CD1-B0F2-5BDFA450284D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-300" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dati generali" sheetId="4" r:id="rId1"/>
+    <sheet name="DatiGenerali" sheetId="4" r:id="rId1"/>
     <sheet name="Misurazioni" sheetId="2" r:id="rId2"/>
     <sheet name="Grafico" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -1234,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF3B858-B44E-4ACE-8F25-54A412D81C95}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,7 +1263,7 @@
   <dimension ref="F1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="C2:E4"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26ADF7C-3EEE-44EB-BC6C-C3F011005C33}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aggiunto supporto per tab diverse per apertura e chiusura valvola. Ora è stata modificata solo la libreria. Non ancora base.xslt
</commit_message>
<xml_diff>
--- a/ProgettoFormLetturaDati/HydrogenOMB/bin/Debug/File/base.xlsx
+++ b/ProgettoFormLetturaDati/HydrogenOMB/bin/Debug/File/base.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\principale\source\repos\ProgettoOMBCorreggiuto\ProgettoFormLetturaDati\HydrogenOMB\bin\Debug\File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\source\repos\ProgettoOMB\ProgettoFormLetturaDati\HydrogenOMB\bin\Debug\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58CCC76-A87D-4CD1-B0F2-5BDFA450284D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6706B83A-10AF-40CC-9335-D015C4911281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatiGenerali" sheetId="4" r:id="rId1"/>
-    <sheet name="Misurazioni" sheetId="2" r:id="rId2"/>
-    <sheet name="Grafico" sheetId="3" r:id="rId3"/>
+    <sheet name="MisurazioniApertura" sheetId="2" r:id="rId2"/>
+    <sheet name="MisurazioniChiusura" sheetId="5" r:id="rId3"/>
+    <sheet name="Grafico" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Angolo">OFFSET(Misurazioni!$C$2,0,0,Misurazioni!$F$1)</definedName>
-    <definedName name="Trimmer">OFFSET(Misurazioni!$D$2,0,0,Misurazioni!$F$1)</definedName>
+    <definedName name="Angolo">OFFSET(MisurazioniApertura!$C$2,0,0,MisurazioniApertura!$F$1)</definedName>
+    <definedName name="Trimmer">OFFSET(MisurazioniApertura!$D$2,0,0,MisurazioniApertura!$F$1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,8 +34,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1262,9 +1263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669F6F74-513D-4C94-B6DE-E93AC5E8854B}">
   <dimension ref="F1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1286,6 +1285,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E58275-41A7-4F03-A451-BBB72D77F0A2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26ADF7C-3EEE-44EB-BC6C-C3F011005C33}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Aggiornato base.xslt e ora i calcoli sono disabilitati in tutto il file excel
</commit_message>
<xml_diff>
--- a/ProgettoFormLetturaDati/HydrogenOMB/bin/Debug/File/base.xlsx
+++ b/ProgettoFormLetturaDati/HydrogenOMB/bin/Debug/File/base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\source\repos\ProgettoOMB\ProgettoFormLetturaDati\HydrogenOMB\bin\Debug\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6706B83A-10AF-40CC-9335-D015C4911281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D8AC135-BFF8-4BE4-8D4E-C7D7998856A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatiGenerali" sheetId="4" r:id="rId1"/>
@@ -19,24 +19,16 @@
     <sheet name="Grafico" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Angolo">OFFSET(MisurazioniApertura!$C$2,0,0,MisurazioniApertura!$F$1)</definedName>
-    <definedName name="Trimmer">OFFSET(MisurazioniApertura!$D$2,0,0,MisurazioniApertura!$F$1)</definedName>
+    <definedName name="AngoloApertura">OFFSET(MisurazioniApertura!$C$2,0,0,MisurazioniApertura!$F$1)</definedName>
+    <definedName name="AngoloChiusura">OFFSET(MisurazioniChiusura!$C$2,0,0,MisurazioniChiusura!$F$1)</definedName>
+    <definedName name="TrimmerApertura">OFFSET(MisurazioniApertura!$D$2,0,0,MisurazioniApertura!$F$1)</definedName>
+    <definedName name="TrimmerChiusura">OFFSET(MisurazioniChiusura!$D$2,0,0,MisurazioniChiusura!$F$1)</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -134,7 +126,62 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Grafico Apertura</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -169,7 +216,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>[0]!Trimmer</c:f>
+              <c:f>[0]!TrimmerApertura</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -184,20 +231,20 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
-                  <c:multiLvlStrRef>
+                  <c:numRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[0]!Angolo</c15:sqref>
+                          <c15:sqref>[0]!AngoloApertura</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
-                  </c:multiLvlStrRef>
+                  </c:numRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-257B-4057-B618-58944744A0B8}"/>
+              <c16:uniqueId val="{00000004-FF4C-4A13-9BFF-98590DC602B7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -211,11 +258,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="443017768"/>
-        <c:axId val="443013808"/>
+        <c:axId val="372089936"/>
+        <c:axId val="372084360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="443017768"/>
+        <c:axId val="372089936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -243,7 +290,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="sng" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -258,7 +305,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443013808"/>
+        <c:crossAx val="372084360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -266,7 +313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443013808"/>
+        <c:axId val="372084360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -302,7 +349,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="sng" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -317,9 +364,9 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443017768"/>
+        <c:crossAx val="372089936"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -360,7 +407,320 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr u="sng"/>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Grafico</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> Chiusura</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>[0]!TrimmerChiusura</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[0]!AngoloChiusura</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                  </c:numRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-406C-459A-B831-B4DA454C5547}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="371400416"/>
+        <c:axId val="371403696"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="371400416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="371403696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="371403696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="371400416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
       </a:pPr>
       <a:endParaRPr lang="it-IT"/>
     </a:p>
@@ -413,8 +773,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -522,11 +922,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -537,11 +932,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -573,9 +963,509 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -933,23 +1823,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3174</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>3174</xdr:rowOff>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>31749</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="2" name="Grafico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D7220FF-90E2-38E6-CD5A-A82FD31F580F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9047FF0-1D53-4906-828B-F7AAD1BFD7B9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -962,6 +1852,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F5F98F9-C743-41E0-9612-C509426ABF66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1235,7 +2161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF3B858-B44E-4ACE-8F25-54A412D81C95}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1261,7 +2187,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669F6F74-513D-4C94-B6DE-E93AC5E8854B}">
-  <dimension ref="F1:F5"/>
+  <dimension ref="C1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="1">
+        <f>COUNT(C:C)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E58275-41A7-4F03-A451-BBB72D77F0A2}">
+  <dimension ref="F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1273,25 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F2" s="1"/>
-    </row>
-    <row r="5" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F5" s="2"/>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E58275-41A7-4F03-A451-BBB72D77F0A2}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1300,12 +2235,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26ADF7C-3EEE-44EB-BC6C-C3F011005C33}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>